<commit_message>
fixed some missing sites
</commit_message>
<xml_diff>
--- a/database/data_to_add/added/2020-06-04/Mathur_1973_tbl1.xlsx
+++ b/database/data_to_add/added/2020-06-04/Mathur_1973_tbl1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacif\Desktop\Project\Extracted\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff.Wesner\Documents\GitHub\Freshwater-Fish-Diet-Database\database\data_to_add\added\2020-06-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E811701-7244-431B-B39E-398FB1728641}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A934130-F6E3-486E-9D66-0F933B3C158D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="45">
   <si>
     <t>site_name</t>
   </si>
@@ -548,7 +548,7 @@
   <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,6 +1232,18 @@
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E9" s="4">
         <v>31</v>
       </c>

</xml_diff>